<commit_message>
Update README.md and change solar app values
</commit_message>
<xml_diff>
--- a/bq25570SolarAppDesignExample_V1p3.xlsx
+++ b/bq25570SolarAppDesignExample_V1p3.xlsx
@@ -1060,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1195,22 +1195,22 @@
         <v>25.755166931637518</v>
       </c>
       <c r="F7" s="6">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G7" s="6">
         <v>60</v>
       </c>
       <c r="H7" s="3">
         <f>24*F7/G7</f>
-        <v>0.11999999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="I7" s="3">
         <f>H7*E7</f>
-        <v>3.0906200317965018</v>
+        <v>10.302066772655008</v>
       </c>
       <c r="J7" s="3">
         <f>I7*$E$3</f>
-        <v>11.435294117647057</v>
+        <v>38.117647058823536</v>
       </c>
       <c r="K7" s="29"/>
     </row>
@@ -1290,14 +1290,14 @@
         <v>0</v>
       </c>
       <c r="F11" s="6">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G11" s="6">
         <v>60</v>
       </c>
       <c r="H11" s="3">
         <f>24*F11/G11</f>
-        <v>0.11999999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="I11" s="3">
         <f>H11*E11</f>
@@ -1336,15 +1336,15 @@
       <c r="G13" s="40"/>
       <c r="H13" s="3">
         <f>24-H7-H11</f>
-        <v>23.759999999999998</v>
+        <v>23.200000000000003</v>
       </c>
       <c r="I13" s="3">
         <f>H13*E13</f>
-        <v>2.3759999999999999</v>
+        <v>2.3200000000000003</v>
       </c>
       <c r="J13" s="3">
         <f>I13*$E$3</f>
-        <v>8.7911999999999999</v>
+        <v>8.5840000000000014</v>
       </c>
       <c r="K13" s="29" t="s">
         <v>20</v>
@@ -1415,7 +1415,7 @@
       <c r="H17" s="48"/>
       <c r="I17" s="23">
         <f>SUM(I7:I15)</f>
-        <v>5.7066200317965023</v>
+        <v>12.862066772655009</v>
       </c>
       <c r="J17" s="20" t="s">
         <v>19</v>
@@ -1433,7 +1433,7 @@
       <c r="G18" s="45"/>
       <c r="H18" s="45"/>
       <c r="I18" s="15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J18" s="20" t="s">
         <v>30</v>
@@ -1452,7 +1452,7 @@
       <c r="H19" s="44"/>
       <c r="I19" s="7">
         <f>I17*I18</f>
-        <v>22.826480127186009</v>
+        <v>38.586200317965023</v>
       </c>
       <c r="J19" s="20" t="s">
         <v>0</v>
@@ -1539,7 +1539,7 @@
       <c r="H23" s="37"/>
       <c r="I23" s="26">
         <f>2*I19/1000*3600*E3/(I22^2-I21^2)</f>
-        <v>62.368967239819007</v>
+        <v>105.42937194570135</v>
       </c>
       <c r="J23" s="20" t="s">
         <v>22</v>
@@ -1573,7 +1573,7 @@
       <c r="I25" s="58"/>
       <c r="J25" s="3">
         <f>SUM(J7:J15)</f>
-        <v>21.114494117647059</v>
+        <v>47.589647058823537</v>
       </c>
       <c r="K25" t="s">
         <v>18</v>
@@ -1610,7 +1610,7 @@
       <c r="I27" s="58"/>
       <c r="J27" s="3">
         <f>J25*J26</f>
-        <v>147.8014588235294</v>
+        <v>333.12752941176478</v>
       </c>
       <c r="K27" t="s">
         <v>53</v>
@@ -1629,7 +1629,7 @@
       <c r="I28" s="55"/>
       <c r="J28" s="3">
         <f>J26-I18</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K28" t="s">
         <v>30</v>
@@ -1651,7 +1651,7 @@
       <c r="I29" s="58"/>
       <c r="J29" s="3">
         <f>J27/J28</f>
-        <v>49.267152941176469</v>
+        <v>83.281882352941196</v>
       </c>
       <c r="K29" t="s">
         <v>18</v>
@@ -1695,7 +1695,7 @@
       <c r="I31" s="37"/>
       <c r="J31" s="3">
         <f>J29/J30</f>
-        <v>6.1583941176470587</v>
+        <v>10.410235294117649</v>
       </c>
       <c r="K31" t="s">
         <v>4</v>
@@ -1742,7 +1742,7 @@
       <c r="I34" s="44"/>
       <c r="J34" s="7">
         <f>J31/J33</f>
-        <v>7.6979926470588227</v>
+        <v>13.012794117647061</v>
       </c>
       <c r="K34" t="s">
         <v>4</v>
@@ -1772,7 +1772,7 @@
       <c r="H36" s="38"/>
       <c r="I36" s="38"/>
       <c r="J36" s="15">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K36" t="s">
         <v>14</v>
@@ -1794,7 +1794,7 @@
       <c r="I37" s="49"/>
       <c r="J37" s="7">
         <f>J34/J36</f>
-        <v>15.395985294117645</v>
+        <v>16.265992647058827</v>
       </c>
       <c r="K37" t="s">
         <v>15</v>

</xml_diff>